<commit_message>
Add two testcases register
</commit_message>
<xml_diff>
--- a/checkList_aliexpress.xlsx
+++ b/checkList_aliexpress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myFolders\Artefacts\forThePortfolio\aliexpressTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB7ADA7-D3E3-46E0-9F68-903DA9CE32F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999E7579-58C7-4999-9CC2-10340E605473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2049224E-37F7-43BF-A8FD-B073BBD39D05}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{2049224E-37F7-43BF-A8FD-B073BBD39D05}"/>
   </bookViews>
   <sheets>
     <sheet name="checklist_sing_in" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="191">
   <si>
     <t xml:space="preserve"> 27.12.2022 18:44           </t>
   </si>
@@ -635,6 +635,66 @@
   </si>
   <si>
     <t>Скрыть / показать</t>
+  </si>
+  <si>
+    <t>Регистрация нового пользователя</t>
+  </si>
+  <si>
+    <t>email: dimatestov@gmail.com
+password: 123456Love</t>
+  </si>
+  <si>
+    <t>1. Окно регистрации открывается
+2. Выпадающий список стран открывается. Локация Турция доступна для выбора
+3. Введенные данные отображаются в полях
+4. Аккаунт создается
+5. Слайдер перетаскивается
+6. Письмо на почту приходит
+7. Код отображается
+8. Email подтверждается
+9. Пользователь активен</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регистрация по email несуществующего пользователя </t>
+  </si>
+  <si>
+    <t>email: testdim@gmail.com
+password: 123456Love</t>
+  </si>
+  <si>
+    <t>1. Открыть Профиль &gt; Регистрация
+2. Выбрать локацию Турция
+3. Ввести тестовые данные в соответствующие поля
+4. Нажать создать аккаунт
+5. Перетащить слайдер вправо
+6. Проверить почту
+7. Ввести проверочный код  
+8. Нажать подтвердить email 
+9. Ввойти в систему</t>
+  </si>
+  <si>
+    <t>1_REG</t>
+  </si>
+  <si>
+    <t>2_REG</t>
+  </si>
+  <si>
+    <t>1. Email был создан
+2. Пользователь не зарегестрирован в системе
+3. Открыть https://best.aliexpress.com/</t>
+  </si>
+  <si>
+    <t>1. Открыть Профиль &gt; Регистрация
+2. Выбрать локацию Турция
+3. Ввести тестовые данные в соответствующие поля
+4. Нажать создать аккаунт
+5. Перетащить слайдер вправо
+6. Проверить почту
+7. Ввести проверочный код  
+8. Нажать подтвердить email 
+9. Ввойти в систем
+10. Нажать Выйти из системы
+11. Войти в систему с учетными данными пользователя</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1168,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1168,24 +1228,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="9" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1204,72 +1246,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1279,24 +1264,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1305,24 +1278,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1370,24 +1325,143 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1724,7 +1798,7 @@
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="25" t="s">
         <v>132</v>
       </c>
       <c r="C1" s="14"/>
@@ -1781,16 +1855,16 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:11" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="27" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="23" t="s">
@@ -1801,58 +1875,58 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="29" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="75"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="36" t="s">
+      <c r="A8" s="65"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="75"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="36" t="s">
+      <c r="A9" s="65"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="30" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="75"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="36" t="s">
+      <c r="A10" s="65"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="30" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="75"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="36" t="s">
+      <c r="A11" s="65"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="75"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="36" t="s">
+      <c r="A12" s="65"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="30" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="15"/>
@@ -1860,10 +1934,10 @@
       <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="75"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39" t="s">
+      <c r="A13" s="65"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="31" t="s">
         <v>57</v>
       </c>
       <c r="E13" s="4"/>
@@ -1873,10 +1947,10 @@
       <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="75"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="36" t="s">
+      <c r="A14" s="65"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="30" t="s">
         <v>59</v>
       </c>
       <c r="E14" s="4"/>
@@ -1886,10 +1960,10 @@
       <c r="K14" s="16"/>
     </row>
     <row r="15" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="75"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="40" t="s">
+      <c r="A15" s="65"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="90" t="s">
         <v>58</v>
       </c>
       <c r="E15" s="4"/>
@@ -1899,10 +1973,10 @@
       <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="75"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="91"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="I16" s="15"/>
@@ -1910,12 +1984,12 @@
       <c r="K16" s="16"/>
     </row>
     <row r="17" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="75"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="43" t="s">
+      <c r="A17" s="65"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="32" t="s">
         <v>62</v>
       </c>
       <c r="E17" s="4"/>
@@ -1925,10 +1999,10 @@
       <c r="K17" s="16"/>
     </row>
     <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="75"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="36" t="s">
+      <c r="A18" s="65"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="30" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="4"/>
@@ -1938,32 +2012,32 @@
       <c r="K18" s="16"/>
     </row>
     <row r="19" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="75"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="36" t="s">
+      <c r="A19" s="65"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="30" t="s">
         <v>64</v>
       </c>
       <c r="I19" s="15"/>
-      <c r="J19" s="30"/>
+      <c r="J19" s="76"/>
       <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="75"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="36" t="s">
+      <c r="A20" s="65"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="30" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="15"/>
-      <c r="J20" s="30"/>
+      <c r="J20" s="76"/>
       <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="75"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="36" t="s">
+      <c r="A21" s="65"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="30" t="s">
         <v>67</v>
       </c>
       <c r="I21" s="15"/>
@@ -1971,10 +2045,10 @@
       <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="75"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="36" t="s">
+      <c r="A22" s="65"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="30" t="s">
         <v>14</v>
       </c>
       <c r="I22" s="11"/>
@@ -1982,10 +2056,10 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="75"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="36" t="s">
+      <c r="A23" s="65"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="30" t="s">
         <v>15</v>
       </c>
       <c r="I23" s="11"/>
@@ -1993,330 +2067,330 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="75"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="36" t="s">
+      <c r="A24" s="65"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="36" t="s">
+      <c r="A25" s="65"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="30" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="0.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="75"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="46"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="77"/>
     </row>
     <row r="27" spans="1:11" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="75"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="77"/>
     </row>
     <row r="28" spans="1:11" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="75"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="78"/>
     </row>
     <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="75"/>
-      <c r="B29" s="56" t="s">
+      <c r="A29" s="65"/>
+      <c r="B29" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="59" t="s">
+      <c r="D29" s="34" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="75"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="60" t="s">
+      <c r="A30" s="65"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="35" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="75"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="60" t="s">
+      <c r="A31" s="65"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="35" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="75"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="60" t="s">
+      <c r="A32" s="65"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="35" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="75"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="60" t="s">
+      <c r="A33" s="65"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="35" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="75"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="60" t="s">
+      <c r="A34" s="65"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="35" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="75"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="60" t="s">
+      <c r="A35" s="65"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="35" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="75"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="60" t="s">
+      <c r="A36" s="65"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="35" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="75"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="60" t="s">
+      <c r="A37" s="65"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="75"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="61" t="s">
+      <c r="A38" s="65"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="36" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="75"/>
-      <c r="B39" s="62" t="s">
+      <c r="A39" s="65"/>
+      <c r="B39" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C39" s="88" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="64" t="s">
+      <c r="D39" s="37" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="75"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="36" t="s">
+      <c r="A40" s="65"/>
+      <c r="B40" s="86"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="30" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="75"/>
-      <c r="B41" s="65"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="36" t="s">
+      <c r="A41" s="65"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="30" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="75"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="36" t="s">
+      <c r="A42" s="65"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="30" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="75"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="26" t="s">
+      <c r="A43" s="65"/>
+      <c r="B43" s="86"/>
+      <c r="C43" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="36" t="s">
+      <c r="D43" s="30" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="75"/>
-      <c r="B44" s="65"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="36" t="s">
+      <c r="A44" s="65"/>
+      <c r="B44" s="86"/>
+      <c r="C44" s="94"/>
+      <c r="D44" s="30" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="75"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="36" t="s">
+      <c r="A45" s="65"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="94"/>
+      <c r="D45" s="30" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="75"/>
-      <c r="B46" s="65"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="36" t="s">
+      <c r="A46" s="65"/>
+      <c r="B46" s="86"/>
+      <c r="C46" s="94"/>
+      <c r="D46" s="30" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="75"/>
-      <c r="B47" s="65"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="36" t="s">
+      <c r="A47" s="65"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="30" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A48" s="75"/>
-      <c r="B48" s="65"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="66" t="s">
+      <c r="A48" s="65"/>
+      <c r="B48" s="86"/>
+      <c r="C48" s="94"/>
+      <c r="D48" s="38" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="75"/>
-      <c r="B49" s="67"/>
-      <c r="C49" s="68" t="s">
+      <c r="A49" s="65"/>
+      <c r="B49" s="87"/>
+      <c r="C49" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="69" t="s">
+      <c r="D49" s="40" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="75"/>
-      <c r="B50" s="62" t="s">
+      <c r="A50" s="65"/>
+      <c r="B50" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="63" t="s">
+      <c r="C50" s="88" t="s">
         <v>94</v>
       </c>
-      <c r="D50" s="64" t="s">
+      <c r="D50" s="37" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="75"/>
-      <c r="B51" s="65"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="70" t="s">
+      <c r="A51" s="65"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="41" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="75"/>
-      <c r="B52" s="65"/>
-      <c r="C52" s="28" t="s">
+      <c r="A52" s="65"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="D52" s="36" t="s">
+      <c r="D52" s="30" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="75"/>
-      <c r="B53" s="65"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="70" t="s">
+      <c r="A53" s="65"/>
+      <c r="B53" s="86"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="41" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="75"/>
-      <c r="B54" s="65"/>
-      <c r="C54" s="27" t="s">
+      <c r="A54" s="65"/>
+      <c r="B54" s="86"/>
+      <c r="C54" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D54" s="30" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="75"/>
-      <c r="B55" s="65"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="70" t="s">
+      <c r="A55" s="65"/>
+      <c r="B55" s="86"/>
+      <c r="C55" s="89"/>
+      <c r="D55" s="41" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="75"/>
-      <c r="B56" s="65"/>
-      <c r="C56" s="27" t="s">
+      <c r="A56" s="65"/>
+      <c r="B56" s="86"/>
+      <c r="C56" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="36" t="s">
+      <c r="D56" s="30" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="75"/>
-      <c r="B57" s="67"/>
-      <c r="C57" s="71"/>
-      <c r="D57" s="69" t="s">
+      <c r="A57" s="65"/>
+      <c r="B57" s="87"/>
+      <c r="C57" s="96"/>
+      <c r="D57" s="40" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="75"/>
-      <c r="B58" s="62" t="s">
+      <c r="A58" s="65"/>
+      <c r="B58" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="72" t="s">
+      <c r="C58" s="92" t="s">
         <v>100</v>
       </c>
-      <c r="D58" s="44" t="s">
+      <c r="D58" s="32" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="75"/>
-      <c r="B59" s="67"/>
-      <c r="C59" s="73"/>
-      <c r="D59" s="49" t="s">
+      <c r="A59" s="65"/>
+      <c r="B59" s="87"/>
+      <c r="C59" s="93"/>
+      <c r="D59" s="33" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="75"/>
-      <c r="B60" s="62" t="s">
+      <c r="A60" s="65"/>
+      <c r="B60" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C60" s="72" t="s">
+      <c r="C60" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="D60" s="64" t="s">
+      <c r="D60" s="37" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="76"/>
-      <c r="B61" s="67"/>
-      <c r="C61" s="73"/>
-      <c r="D61" s="49" t="s">
+      <c r="A61" s="66"/>
+      <c r="B61" s="87"/>
+      <c r="C61" s="93"/>
+      <c r="D61" s="33" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2499,6 +2573,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B50:B57"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
     <mergeCell ref="A7:A61"/>
     <mergeCell ref="B7:B28"/>
     <mergeCell ref="C7:C16"/>
@@ -2515,11 +2594,6 @@
     <mergeCell ref="B60:B61"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C43:C48"/>
-    <mergeCell ref="B50:B57"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{9C309FA4-95D4-4D0F-BEEE-98B6E643D90B}"/>
@@ -2539,214 +2613,214 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="84"/>
-    <col min="2" max="2" width="37" style="84" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="84" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="84" customWidth="1"/>
-    <col min="5" max="5" width="42.109375" style="81" customWidth="1"/>
-    <col min="6" max="6" width="31.44140625" style="84" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="49"/>
+    <col min="2" max="2" width="37" style="49" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="49" customWidth="1"/>
+    <col min="5" max="5" width="42.109375" style="46" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" style="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="45" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="83" t="s">
+      <c r="D2" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E2" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="90" t="s">
+      <c r="F2" s="55" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="55" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="F4" s="55" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="83" t="s">
+      <c r="E5" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="90" t="s">
+      <c r="F5" s="55" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="90" t="s">
+      <c r="F6" s="55" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="83" t="s">
+      <c r="E7" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="F7" s="90" t="s">
+      <c r="F7" s="55" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="83" t="s">
+      <c r="E8" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="F8" s="90" t="s">
+      <c r="F8" s="55" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="93" t="s">
+      <c r="E9" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="59" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="86"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="88"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="53"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="81"/>
-      <c r="F11" s="85"/>
+      <c r="A11" s="46"/>
+      <c r="F11" s="50"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F12" s="85"/>
+      <c r="F12" s="50"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F13" s="85"/>
+      <c r="F13" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2758,7 +2832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD47D6E4-C312-4AC1-B2DF-FA1217C956A1}">
   <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" zoomScaleSheetLayoutView="123" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="123" workbookViewId="0">
       <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
@@ -2775,7 +2849,7 @@
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="25" t="s">
         <v>131</v>
       </c>
       <c r="C1" s="14"/>
@@ -2832,16 +2906,16 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="27" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="23" t="s">
@@ -2852,13 +2926,13 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="100" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="89" t="s">
         <v>130</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -2868,41 +2942,41 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="101"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="27"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="89"/>
       <c r="D8" s="19" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="101"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="27"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="19" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="101"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="99"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="89"/>
       <c r="D10" s="19" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="101"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="27"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="89"/>
       <c r="D11" s="19" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="101"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="99"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="19" t="s">
         <v>138</v>
       </c>
@@ -2911,9 +2985,9 @@
       <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="101"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="99"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="89"/>
       <c r="D13" s="19" t="s">
         <v>139</v>
       </c>
@@ -2924,9 +2998,9 @@
       <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="101"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="27"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="89"/>
       <c r="D14" s="18" t="s">
         <v>140</v>
       </c>
@@ -2937,11 +3011,11 @@
       <c r="K14" s="16"/>
     </row>
     <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="101"/>
-      <c r="B15" s="25" t="s">
+      <c r="A15" s="99"/>
+      <c r="B15" s="98" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="89" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="19" t="s">
@@ -2954,9 +3028,9 @@
       <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="101"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="99"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="89"/>
       <c r="D16" s="20" t="s">
         <v>144</v>
       </c>
@@ -2967,9 +3041,9 @@
       <c r="K16" s="16"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="101"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="27"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="89"/>
       <c r="D17" s="21" t="s">
         <v>136</v>
       </c>
@@ -2980,9 +3054,9 @@
       <c r="K17" s="16"/>
     </row>
     <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="101"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="27"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="98"/>
+      <c r="C18" s="89"/>
       <c r="D18" s="19" t="s">
         <v>146</v>
       </c>
@@ -2993,31 +3067,31 @@
       <c r="K18" s="16"/>
     </row>
     <row r="19" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="101"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="27"/>
+      <c r="A19" s="99"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="89"/>
       <c r="D19" s="19" t="s">
         <v>147</v>
       </c>
       <c r="I19" s="15"/>
-      <c r="J19" s="30"/>
+      <c r="J19" s="76"/>
       <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="101"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="27"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="89"/>
       <c r="D20" s="19" t="s">
         <v>148</v>
       </c>
       <c r="I20" s="15"/>
-      <c r="J20" s="30"/>
+      <c r="J20" s="76"/>
       <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="101"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="27"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="89"/>
       <c r="D21" s="19" t="s">
         <v>149</v>
       </c>
@@ -3026,9 +3100,9 @@
       <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="101"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="27"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="89"/>
       <c r="D22" s="19" t="s">
         <v>150</v>
       </c>
@@ -3037,9 +3111,9 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="101"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="27"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="89"/>
       <c r="D23" s="19" t="s">
         <v>140</v>
       </c>
@@ -3048,49 +3122,49 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="101"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="27"/>
+      <c r="A24" s="99"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="89"/>
       <c r="D24" s="19" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="101"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="27"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="89"/>
       <c r="D25" s="19" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="0.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="101"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="32" t="s">
+      <c r="A26" s="99"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="26" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="101"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="32" t="s">
+      <c r="A27" s="99"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="26" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="101"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="27"/>
+      <c r="A28" s="99"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="89"/>
       <c r="D28" s="21" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="101"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="27" t="s">
+      <c r="A29" s="99"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="89" t="s">
         <v>61</v>
       </c>
       <c r="D29" s="21" t="s">
@@ -3098,107 +3172,107 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="101"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="27"/>
+      <c r="A30" s="99"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="89"/>
       <c r="D30" s="19" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="101"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="27"/>
+      <c r="A31" s="99"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="89"/>
       <c r="D31" s="19" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="101"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="27"/>
+      <c r="A32" s="99"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="89"/>
       <c r="D32" s="19" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="101"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="27"/>
+      <c r="A33" s="99"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="89"/>
       <c r="D33" s="19" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="101"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="27"/>
+      <c r="A34" s="99"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="89"/>
       <c r="D34" s="19" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="101"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="27"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="89"/>
       <c r="D35" s="19" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="101"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="27"/>
+      <c r="A36" s="99"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="89"/>
       <c r="D36" s="19" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="101"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="27"/>
+      <c r="A37" s="99"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="89"/>
       <c r="D37" s="19" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="101"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="27"/>
+      <c r="A38" s="99"/>
+      <c r="B38" s="98"/>
+      <c r="C38" s="89"/>
       <c r="D38" s="19" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="101"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="27"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="89"/>
       <c r="D39" s="19" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="101"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="27"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="89"/>
       <c r="D40" s="19" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="101"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="27"/>
+      <c r="A41" s="99"/>
+      <c r="B41" s="98"/>
+      <c r="C41" s="89"/>
       <c r="D41" s="19" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="101"/>
-      <c r="B42" s="25" t="s">
+      <c r="A42" s="99"/>
+      <c r="B42" s="98" t="s">
         <v>163</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="89" t="s">
         <v>164</v>
       </c>
       <c r="D42" s="19" t="s">
@@ -3206,59 +3280,59 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="101"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="27"/>
+      <c r="A43" s="99"/>
+      <c r="B43" s="98"/>
+      <c r="C43" s="89"/>
       <c r="D43" s="19" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="101"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="27"/>
+      <c r="A44" s="99"/>
+      <c r="B44" s="98"/>
+      <c r="C44" s="89"/>
       <c r="D44" s="19" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="101"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="27"/>
+      <c r="A45" s="99"/>
+      <c r="B45" s="98"/>
+      <c r="C45" s="89"/>
       <c r="D45" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="101"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="27"/>
+      <c r="A46" s="99"/>
+      <c r="B46" s="98"/>
+      <c r="C46" s="89"/>
       <c r="D46" s="19" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="101"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="27"/>
+      <c r="A47" s="99"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="89"/>
       <c r="D47" s="19" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="101"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="27"/>
+      <c r="A48" s="99"/>
+      <c r="B48" s="98"/>
+      <c r="C48" s="89"/>
       <c r="D48" s="19" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="101"/>
-      <c r="B49" s="25" t="s">
+      <c r="A49" s="99"/>
+      <c r="B49" s="98" t="s">
         <v>169</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="89" t="s">
         <v>170</v>
       </c>
       <c r="D49" s="19" t="s">
@@ -3266,25 +3340,25 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="101"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="27"/>
+      <c r="A50" s="99"/>
+      <c r="B50" s="98"/>
+      <c r="C50" s="89"/>
       <c r="D50" s="19" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="101"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="27"/>
+      <c r="A51" s="99"/>
+      <c r="B51" s="98"/>
+      <c r="C51" s="89"/>
       <c r="D51" s="21" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="101"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="28" t="s">
+      <c r="A52" s="99"/>
+      <c r="B52" s="98"/>
+      <c r="C52" s="95" t="s">
         <v>95</v>
       </c>
       <c r="D52" s="21" t="s">
@@ -3292,17 +3366,17 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="101"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="99"/>
+      <c r="B53" s="98"/>
+      <c r="C53" s="95"/>
       <c r="D53" s="21" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="101"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="27" t="s">
+      <c r="A54" s="99"/>
+      <c r="B54" s="98"/>
+      <c r="C54" s="89" t="s">
         <v>96</v>
       </c>
       <c r="D54" s="19" t="s">
@@ -3310,17 +3384,17 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="101"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="27"/>
+      <c r="A55" s="99"/>
+      <c r="B55" s="98"/>
+      <c r="C55" s="89"/>
       <c r="D55" s="19" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="101"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="27" t="s">
+      <c r="A56" s="99"/>
+      <c r="B56" s="98"/>
+      <c r="C56" s="89" t="s">
         <v>97</v>
       </c>
       <c r="D56" s="19" t="s">
@@ -3328,17 +3402,17 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="101"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="27"/>
+      <c r="A57" s="99"/>
+      <c r="B57" s="98"/>
+      <c r="C57" s="89"/>
       <c r="D57" s="21" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="101"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="27" t="s">
+      <c r="A58" s="99"/>
+      <c r="B58" s="98"/>
+      <c r="C58" s="89" t="s">
         <v>174</v>
       </c>
       <c r="D58" s="21" t="s">
@@ -3346,17 +3420,17 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="101"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="27"/>
+      <c r="A59" s="99"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="89"/>
       <c r="D59" s="21" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="101"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="27" t="s">
+      <c r="A60" s="99"/>
+      <c r="B60" s="98"/>
+      <c r="C60" s="89" t="s">
         <v>94</v>
       </c>
       <c r="D60" s="19" t="s">
@@ -3364,17 +3438,17 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="101"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="27"/>
+      <c r="A61" s="99"/>
+      <c r="B61" s="98"/>
+      <c r="C61" s="89"/>
       <c r="D61" s="21" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="101"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="95" t="s">
+      <c r="A62" s="99"/>
+      <c r="B62" s="98"/>
+      <c r="C62" s="97" t="s">
         <v>176</v>
       </c>
       <c r="D62" s="19" t="s">
@@ -3382,16 +3456,16 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="101"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="95"/>
+      <c r="A63" s="99"/>
+      <c r="B63" s="98"/>
+      <c r="C63" s="97"/>
       <c r="D63" s="21" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="101"/>
-      <c r="B64" s="25"/>
+      <c r="A64" s="99"/>
+      <c r="B64" s="98"/>
       <c r="C64" s="24" t="s">
         <v>179</v>
       </c>
@@ -3400,11 +3474,11 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="101"/>
-      <c r="B65" s="25" t="s">
+      <c r="A65" s="99"/>
+      <c r="B65" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C65" s="94" t="s">
         <v>100</v>
       </c>
       <c r="D65" s="21" t="s">
@@ -3412,19 +3486,19 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="101"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="26"/>
+      <c r="A66" s="99"/>
+      <c r="B66" s="98"/>
+      <c r="C66" s="94"/>
       <c r="D66" s="19" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="101"/>
-      <c r="B67" s="25" t="s">
+      <c r="A67" s="99"/>
+      <c r="B67" s="98" t="s">
         <v>50</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="94" t="s">
         <v>103</v>
       </c>
       <c r="D67" s="19" t="s">
@@ -3432,297 +3506,297 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="101"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="26"/>
+      <c r="A68" s="99"/>
+      <c r="B68" s="98"/>
+      <c r="C68" s="94"/>
       <c r="D68" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="97"/>
-      <c r="B69" s="97"/>
-      <c r="C69" s="99"/>
-      <c r="D69" s="100"/>
+      <c r="A69" s="61"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="63"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="97"/>
-      <c r="B70" s="97"/>
-      <c r="C70" s="99"/>
-      <c r="D70" s="100"/>
+      <c r="A70" s="61"/>
+      <c r="B70" s="61"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="63"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="97"/>
-      <c r="B71" s="97"/>
-      <c r="C71" s="99"/>
-      <c r="D71" s="100"/>
+      <c r="A71" s="61"/>
+      <c r="B71" s="61"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="63"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="97"/>
-      <c r="B72" s="97"/>
-      <c r="C72" s="99"/>
-      <c r="D72" s="100"/>
+      <c r="A72" s="61"/>
+      <c r="B72" s="61"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="63"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="97"/>
-      <c r="B73" s="97"/>
-      <c r="C73" s="99"/>
-      <c r="D73" s="100"/>
+      <c r="A73" s="61"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="63"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="97"/>
-      <c r="B74" s="97"/>
-      <c r="C74" s="99"/>
-      <c r="D74" s="100"/>
+      <c r="A74" s="61"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="63"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="97"/>
-      <c r="B75" s="97"/>
-      <c r="C75" s="99"/>
-      <c r="D75" s="100"/>
+      <c r="A75" s="61"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="63"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="97"/>
-      <c r="B76" s="97"/>
-      <c r="C76" s="99"/>
-      <c r="D76" s="100"/>
+      <c r="A76" s="61"/>
+      <c r="B76" s="61"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="63"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="97"/>
-      <c r="B77" s="97"/>
-      <c r="C77" s="99"/>
-      <c r="D77" s="100"/>
+      <c r="A77" s="61"/>
+      <c r="B77" s="61"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="63"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="97"/>
-      <c r="B78" s="97"/>
-      <c r="C78" s="99"/>
-      <c r="D78" s="100"/>
+      <c r="A78" s="61"/>
+      <c r="B78" s="61"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="63"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="97"/>
-      <c r="B79" s="97"/>
-      <c r="C79" s="99"/>
-      <c r="D79" s="100"/>
+      <c r="A79" s="61"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="63"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="97"/>
-      <c r="B80" s="97"/>
-      <c r="C80" s="99"/>
-      <c r="D80" s="99"/>
+      <c r="A80" s="61"/>
+      <c r="B80" s="61"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="96"/>
+      <c r="A81" s="60"/>
       <c r="B81" s="11"/>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="96"/>
+      <c r="A82" s="60"/>
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="96"/>
+      <c r="A83" s="60"/>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="96"/>
+      <c r="A84" s="60"/>
       <c r="B84" s="11"/>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="96"/>
+      <c r="A85" s="60"/>
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="96"/>
+      <c r="A86" s="60"/>
       <c r="B86" s="11"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="96"/>
+      <c r="A87" s="60"/>
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="96"/>
+      <c r="A88" s="60"/>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="96"/>
+      <c r="A89" s="60"/>
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="96"/>
+      <c r="A90" s="60"/>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="96"/>
+      <c r="A91" s="60"/>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="96"/>
+      <c r="A92" s="60"/>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="96"/>
+      <c r="A93" s="60"/>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="96"/>
+      <c r="A94" s="60"/>
       <c r="B94" s="11"/>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="96"/>
+      <c r="A95" s="60"/>
       <c r="B95" s="11"/>
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="96"/>
+      <c r="A96" s="60"/>
       <c r="B96" s="11"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="96"/>
+      <c r="A97" s="60"/>
       <c r="B97" s="11"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="96"/>
+      <c r="A98" s="60"/>
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" s="96"/>
+      <c r="A99" s="60"/>
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="96"/>
+      <c r="A100" s="60"/>
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="96"/>
+      <c r="A101" s="60"/>
       <c r="B101" s="11"/>
       <c r="C101" s="11"/>
       <c r="D101" s="11"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="96"/>
+      <c r="A102" s="60"/>
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="96"/>
+      <c r="A103" s="60"/>
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" s="96"/>
+      <c r="A104" s="60"/>
       <c r="B104" s="11"/>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="96"/>
+      <c r="A105" s="60"/>
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="96"/>
+      <c r="A106" s="60"/>
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" s="96"/>
+      <c r="A107" s="60"/>
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="96"/>
+      <c r="A108" s="60"/>
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="96"/>
+      <c r="A109" s="60"/>
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="96"/>
+      <c r="A110" s="60"/>
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="96"/>
+      <c r="A111" s="60"/>
       <c r="B111" s="11"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="96"/>
+      <c r="A112" s="60"/>
       <c r="B112" s="11"/>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" s="96"/>
+      <c r="A113" s="60"/>
       <c r="B113" s="11"/>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" s="96"/>
+      <c r="A114" s="60"/>
       <c r="B114" s="11"/>
       <c r="C114" s="11"/>
       <c r="D114" s="11"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" s="96"/>
+      <c r="A115" s="60"/>
       <c r="B115" s="11"/>
       <c r="C115" s="11"/>
       <c r="D115" s="11"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" s="98"/>
+      <c r="A116" s="62"/>
       <c r="B116" s="11"/>
       <c r="C116" s="11"/>
       <c r="D116" s="11"/>
@@ -3747,27 +3821,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C7:C14"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="C15:C28"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A7:A68"/>
+    <mergeCell ref="C29:C41"/>
+    <mergeCell ref="B15:B41"/>
+    <mergeCell ref="C42:C48"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C60:C61"/>
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="B49:B64"/>
     <mergeCell ref="B65:B66"/>
     <mergeCell ref="C65:C66"/>
     <mergeCell ref="B67:B68"/>
     <mergeCell ref="C67:C68"/>
-    <mergeCell ref="A7:A68"/>
-    <mergeCell ref="C29:C41"/>
-    <mergeCell ref="B15:B41"/>
-    <mergeCell ref="C42:C48"/>
-    <mergeCell ref="B42:B48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C7:C14"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="C15:C28"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{036558F5-5A46-4A50-9971-01BAD1A54C29}"/>
@@ -3779,19 +3853,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{452EA627-B5DC-456E-93F3-7F3FF1386646}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" customWidth="1"/>
     <col min="5" max="5" width="31.5546875" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3814,7 +3888,45 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="162" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="105" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="102" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="105" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="105" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="101" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="105" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="104" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="103" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>